<commit_message>
add ProcessLog file and modify the figure display
</commit_message>
<xml_diff>
--- a/Results_ZC/Average_results_Demand_10.xlsx
+++ b/Results_ZC/Average_results_Demand_10.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="FTNC_Average_Demand10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FTNC_Average_Demand101" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,4 +486,72 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC_Average_Demand_10</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2455.274984722344</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13095.80869023837</v>
+      </c>
+      <c r="D2" t="n">
+        <v>630.3256680479443</v>
+      </c>
+      <c r="E2" t="n">
+        <v>31.57236976815668</v>
+      </c>
+      <c r="F2" t="n">
+        <v>16212.98171277687</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify the excel sheet, almost complete
</commit_message>
<xml_diff>
--- a/Results_ZC/Average_results_Demand_10.xlsx
+++ b/Results_ZC/Average_results_Demand_10.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="FTNC_Average_Demand10" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="FTNC_Average_Demand101" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FTNC_Average_Demand102" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FTHC_Average_Demand10" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -554,4 +556,140 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC_Average_Demand_10</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2489.529745747145</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12889.67819330659</v>
+      </c>
+      <c r="D2" t="n">
+        <v>879.0425212515569</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17.60506501503527</v>
+      </c>
+      <c r="F2" t="n">
+        <v>16275.8555262108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTHC_Average_Demand_10</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2559.442964239976</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13023.49297188319</v>
+      </c>
+      <c r="D2" t="n">
+        <v>646.1927526245161</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.417222010433864</v>
+      </c>
+      <c r="F2" t="n">
+        <v>16237.54591075812</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>